<commit_message>
dia 8 - feat: implementar tuning completo (LR, RF, GB, XGB, LGBM) e gerar relatório PDF; docs: atualizar README com novos resultados; fix: otimizar script de treino para reduzir uso de CPU
</commit_message>
<xml_diff>
--- a/reports/model_metrics.xlsx
+++ b/reports/model_metrics.xlsx
@@ -458,81 +458,81 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Logistic Regression</t>
+          <t>Logistic Regression (Tuned)</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9709702993465252</v>
+        <v>0.9755065433601691</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9183673469387755</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="D2" t="n">
-        <v>0.05798969072164949</v>
+        <v>0.8235294117647058</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Random Forest</t>
+          <t>Random Forest (Tuned)</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9684484390970794</v>
+        <v>0.9652347204357263</v>
       </c>
       <c r="C3" t="n">
-        <v>0.826530612244898</v>
+        <v>0.7959183673469388</v>
       </c>
       <c r="D3" t="n">
-        <v>0.8709677419354839</v>
+        <v>0.8764044943820225</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Gradient Boosting</t>
+          <t>Gradient Boosting (Tuned)</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.980964697007109</v>
+        <v>0.9129154739414056</v>
       </c>
       <c r="C4" t="n">
-        <v>0.9183673469387755</v>
+        <v>0.7448979591836735</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1133501259445844</v>
+        <v>0.7604166666666666</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>XGBoost</t>
+          <t>XGBoost (Tuned)</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9800664743950478</v>
+        <v>0.9758012852721281</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8775510204081632</v>
+        <v>0.6938775510204082</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2408963585434174</v>
+        <v>0.8947368421052632</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>LightGBM</t>
+          <t>LightGBM (Tuned)</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.956781773626727</v>
+        <v>0.5479759978696036</v>
       </c>
       <c r="C6" t="n">
-        <v>0.8367346938775511</v>
+        <v>0.173469387755102</v>
       </c>
       <c r="D6" t="n">
-        <v>0.6259541984732825</v>
+        <v>0.08292682926829269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>